<commit_message>
Minor fixes - new line, removing temporal part of code
</commit_message>
<xml_diff>
--- a/example/en_app/xls/E_EN_T2C_authoring.xlsx
+++ b/example/en_app/xls/E_EN_T2C_authoring.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D6DAB8-FCE0-4156-AF95-D1E570F37FFF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F0C64B-A531-42E5-9375-AEAC1FC895D6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="3744" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -250,9 +250,6 @@
     <t xml:space="preserve"> @LIMB</t>
   </si>
   <si>
-    <t>#ACHE &amp;&amp; @LIMB:hand</t>
-  </si>
-  <si>
     <t>Ache of your hand can be an accident</t>
   </si>
   <si>
@@ -272,12 +269,6 @@
   </si>
   <si>
     <t>CT; catscan</t>
-  </si>
-  <si>
-    <t>#WHAT_IS &amp;&amp; @SUBLECT:CT</t>
-  </si>
-  <si>
-    <t>#WHAT_IS &amp;&amp; @SUBLECT:&lt;x&gt;</t>
   </si>
   <si>
     <t>1+1 is 2 %%:b_question</t>
@@ -706,9 +697,6 @@
     <t>X-rays make up X-radiation, a form of electromagnetic radiation.</t>
   </si>
   <si>
-    <t>#WHAT_IS &amp;&amp; @SUBJECT:XRAY</t>
-  </si>
-  <si>
     <t>XRAY; Rontgen</t>
   </si>
   <si>
@@ -770,12 +758,6 @@
   </si>
   <si>
     <t xml:space="preserve">//  in this document we  guide the reader through the format. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> true &amp;&amp; @LIMB:hand</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> true &amp;&amp; @LIMB:leg</t>
   </si>
   <si>
     <t>//This 'true &amp;&amp; ' tweek is added only temporarly overcome the bug of detecting a condition,</t>
@@ -879,6 +861,24 @@
   </si>
   <si>
     <t xml:space="preserve">// The second column is dedicated to output. It contains a plain text or an optional HTML markup. Default client (clientv2) supports HTML formát. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> true and @LIMB:hand</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> true and @LIMB:leg</t>
+  </si>
+  <si>
+    <t>#ACHE and @LIMB:hand</t>
+  </si>
+  <si>
+    <t>#WHAT_IS and @SUBLECT:&lt;x&gt;</t>
+  </si>
+  <si>
+    <t>#WHAT_IS and @SUBLECT:CT</t>
+  </si>
+  <si>
+    <t>#WHAT_IS and @SUBJECT:XRAY</t>
   </si>
 </sst>
 </file>
@@ -1327,10 +1327,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D218"/>
+  <dimension ref="A1:D219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="A178" sqref="A178:XFD179"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="A168" sqref="A168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1347,19 +1347,19 @@
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B3" s="3"/>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1384,7 +1384,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1425,25 +1425,25 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -1475,7 +1475,7 @@
         <v>17</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
@@ -1490,7 +1490,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1523,7 +1523,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1536,22 +1536,22 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -1559,7 +1559,7 @@
         <v>25</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>38</v>
@@ -1571,15 +1571,15 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
@@ -1592,10 +1592,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
@@ -1607,12 +1607,12 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1720,7 +1720,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="68" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -1730,17 +1730,17 @@
     </row>
     <row r="69" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="14" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="14" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="14" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -1748,42 +1748,42 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
@@ -1850,7 +1850,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
@@ -1881,24 +1881,24 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B99" s="8" t="s">
         <v>52</v>
       </c>
       <c r="C99" s="8"/>
       <c r="D99" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B100" s="8"/>
       <c r="C100" s="8"/>
@@ -1906,7 +1906,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B101" s="8"/>
       <c r="C101" s="8"/>
@@ -1920,7 +1920,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B103" s="8"/>
       <c r="C103" s="8"/>
@@ -1931,11 +1931,11 @@
         <v>44</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C104" s="8"/>
       <c r="D104" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
@@ -1949,7 +1949,7 @@
         <v>45</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C106" s="8"/>
       <c r="D106" s="8"/>
@@ -1962,7 +1962,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B108" s="8"/>
       <c r="C108" s="8"/>
@@ -1973,7 +1973,7 @@
         <v>44</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C109" s="8"/>
       <c r="D109" s="8"/>
@@ -1989,24 +1989,24 @@
         <v>45</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C111" s="8"/>
       <c r="D111" s="8"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
@@ -2014,7 +2014,7 @@
         <v>53</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C117" s="8"/>
       <c r="D117" s="8"/>
@@ -2034,17 +2034,17 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="16" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
@@ -2057,7 +2057,7 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B126" s="8"/>
       <c r="C126" s="8"/>
@@ -2065,7 +2065,7 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B127" s="8"/>
       <c r="C127" s="8"/>
@@ -2073,7 +2073,7 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
@@ -2086,17 +2086,17 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C132" s="8"/>
       <c r="D132" s="8"/>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B133" s="8"/>
       <c r="C133" s="8"/>
@@ -2104,75 +2104,67 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="8" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C137" s="8"/>
       <c r="D137" s="8"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A138" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="B138" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C138" s="8"/>
-      <c r="D138" s="8"/>
-    </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A139" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A141" t="s">
-        <v>164</v>
+      <c r="A139" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B139" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C139" s="8"/>
+      <c r="D139" s="8"/>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A144" s="8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A145" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B145" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B144" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C144" s="8"/>
-      <c r="D144" s="8"/>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A146" t="s">
-        <v>166</v>
-      </c>
+      <c r="C145" s="8"/>
+      <c r="D145" s="8"/>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A149" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B149" s="8"/>
-      <c r="C149" s="8"/>
-      <c r="D149" s="8"/>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="8" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B150" s="8"/>
       <c r="C150" s="8"/>
@@ -2180,7 +2172,7 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="8" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B151" s="8"/>
       <c r="C151" s="8"/>
@@ -2195,22 +2187,22 @@
       <c r="D152" s="8"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A153" s="8"/>
+      <c r="A153" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="B153" s="8"/>
       <c r="C153" s="8"/>
       <c r="D153" s="8"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A154" s="8" t="s">
-        <v>63</v>
-      </c>
+      <c r="A154" s="8"/>
       <c r="B154" s="8"/>
       <c r="C154" s="8"/>
       <c r="D154" s="8"/>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B155" s="8"/>
       <c r="C155" s="8"/>
@@ -2218,354 +2210,362 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="8" t="s">
-        <v>157</v>
+        <v>63</v>
       </c>
       <c r="B156" s="8"/>
       <c r="C156" s="8"/>
       <c r="D156" s="8"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A157" s="8"/>
+      <c r="A157" s="8" t="s">
+        <v>153</v>
+      </c>
       <c r="B157" s="8"/>
       <c r="C157" s="8"/>
       <c r="D157" s="8"/>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A158" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="B158" s="8" t="s">
-        <v>153</v>
-      </c>
+      <c r="A158" s="8"/>
+      <c r="B158" s="8"/>
       <c r="C158" s="8"/>
       <c r="D158" s="8"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A159" s="8"/>
-      <c r="B159" s="8"/>
+      <c r="A159" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="B159" s="8" t="s">
+        <v>150</v>
+      </c>
       <c r="C159" s="8"/>
       <c r="D159" s="8"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A160" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="B160" s="8" t="s">
-        <v>155</v>
-      </c>
+      <c r="A160" s="8"/>
+      <c r="B160" s="8"/>
       <c r="C160" s="8"/>
       <c r="D160" s="8"/>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A162" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A164" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B164" s="8"/>
-      <c r="C164" s="8"/>
-      <c r="D164" s="8"/>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A161" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="B161" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C161" s="8"/>
+      <c r="D161" s="8"/>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B165" s="8" t="s">
-        <v>153</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="B165" s="8"/>
       <c r="C165" s="8"/>
       <c r="D165" s="8"/>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" s="8" t="s">
-        <v>154</v>
+        <v>2</v>
       </c>
       <c r="B166" s="8" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C166" s="8"/>
       <c r="D166" s="8"/>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A168" s="14" t="s">
-        <v>129</v>
-      </c>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A167" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B167" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C167" s="8"/>
+      <c r="D167" s="8"/>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" s="14" t="s">
-        <v>189</v>
+        <v>126</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" s="14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A171" s="8" t="s">
+      <c r="A171" s="14" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A172" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B172" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C172" s="8"/>
+      <c r="D172" s="8"/>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A174" s="14" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A176" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B176" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="B171" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="C171" s="8"/>
-      <c r="D171" s="8"/>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A173" s="14" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A175" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="B175" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="C175" s="8"/>
-      <c r="D175" s="8"/>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A176" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="B176" s="14"/>
-    </row>
-    <row r="177" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A178" s="14" t="s">
-        <v>184</v>
-      </c>
-    </row>
+      <c r="C176" s="8"/>
+      <c r="D176" s="8"/>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A177" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="B177" s="14"/>
+    </row>
+    <row r="178" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" s="14" t="s">
-        <v>143</v>
+        <v>178</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" s="14" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" s="14" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" s="14" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" s="14" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" s="14" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" s="14" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" s="14" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" s="14" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" s="14" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" s="14" t="s">
-        <v>71</v>
+        <v>149</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A190" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="B190" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="C190" s="8"/>
-      <c r="D190" s="8"/>
+      <c r="A190" s="14" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A191" s="14" t="s">
-        <v>180</v>
-      </c>
+      <c r="A191" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B191" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C191" s="8"/>
+      <c r="D191" s="8"/>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A192" s="14"/>
+      <c r="A192" s="14" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A193" s="14" t="s">
-        <v>130</v>
-      </c>
+      <c r="A193" s="14"/>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" s="14" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A195" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="B195" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="C195" s="8"/>
-      <c r="D195" s="8"/>
+      <c r="A195" s="14" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A196" s="13"/>
-      <c r="B196" s="13"/>
-      <c r="C196" s="13"/>
-      <c r="D196" s="13"/>
+      <c r="A196" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B196" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C196" s="8"/>
+      <c r="D196" s="8"/>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A197" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="B197" s="13" t="s">
-        <v>139</v>
-      </c>
+      <c r="A197" s="13"/>
+      <c r="B197" s="13"/>
       <c r="C197" s="13"/>
       <c r="D197" s="13"/>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A198" s="13"/>
-      <c r="B198" s="13"/>
+      <c r="A198" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B198" s="13" t="s">
+        <v>136</v>
+      </c>
       <c r="C198" s="13"/>
       <c r="D198" s="13"/>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A199" s="14" t="s">
-        <v>140</v>
-      </c>
+      <c r="A199" s="13"/>
+      <c r="B199" s="13"/>
+      <c r="C199" s="13"/>
+      <c r="D199" s="13"/>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A200" s="14"/>
+      <c r="A200" s="14" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A201" s="14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="202" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A201" s="14"/>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" s="14" t="s">
-        <v>179</v>
+        <v>125</v>
       </c>
     </row>
     <row r="203" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A203" s="14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A204" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="B204" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="C204" s="13"/>
-      <c r="D204" s="13"/>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A205" s="14"/>
+    </row>
+    <row r="204" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A204" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A205" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B205" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="C205" s="13"/>
+      <c r="D205" s="13"/>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A206" s="14" t="s">
-        <v>174</v>
-      </c>
+      <c r="A206" s="14"/>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" s="14" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="208" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A208" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="B208" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="C208" s="13"/>
-      <c r="D208" s="13"/>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A209" s="14"/>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A208" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A209" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="B209" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="C209" s="13"/>
+      <c r="D209" s="13"/>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A210" s="14" t="s">
-        <v>131</v>
-      </c>
+      <c r="A210" s="14"/>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" s="14" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" s="14" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" s="14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A214" s="14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="214" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A214" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="B214" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C214" s="13"/>
-      <c r="D214" s="13"/>
-    </row>
-    <row r="215" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="216" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A216" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B216" s="13"/>
-      <c r="C216" s="13"/>
-      <c r="D216" s="13"/>
-    </row>
+    <row r="215" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A215" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B215" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C215" s="13"/>
+      <c r="D215" s="13"/>
+    </row>
+    <row r="216" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="217" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A217" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="B217" s="13" t="s">
-        <v>70</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="B217" s="13"/>
       <c r="C217" s="13"/>
       <c r="D217" s="13"/>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A218" s="14"/>
+    <row r="218" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A218" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B218" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C218" s="13"/>
+      <c r="D218" s="13"/>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A219" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
use devel version of EN example of xlsx
</commit_message>
<xml_diff>
--- a/example/en_app/xls/E_EN_T2C_authoring.xlsx
+++ b/example/en_app/xls/E_EN_T2C_authoring.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F0C64B-A531-42E5-9375-AEAC1FC895D6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271D0095-5CC0-4B16-AFF2-565287525980}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="3744" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="200">
   <si>
     <t xml:space="preserve"> Je to něco z následujících věcí co vidíte na tlačítkách?</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>CT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">// Označení sekce fakticky reprezentuje jméno prvého uzlu sekce, kde bude probíhat následující krok konverzace a jeho uvedení ve čtvrtém sloupečku znamená že další konverzace má pokračovat tímto uzlem, </t>
   </si>
   <si>
     <r>
@@ -319,21 +316,6 @@
     <t>Let me describe what usually happens further.</t>
   </si>
   <si>
-    <t>// It is not always possible to answer the questions without knowing context. If you want to conduct some steps only if they appear in a particular context, you can describe it in fourth  (D)column by refering to the part, which describes the behivour.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">//   Section is then introduced by opis sekce pak začíná znakem : a stejným jménem </t>
-  </si>
-  <si>
-    <t>// You write the question to the first column (A) . The required answers should be specified in the second column (B)  . Each pair (question, answer) should be separated by empty row</t>
-  </si>
-  <si>
-    <t>// Chat bot described above  is able to answer the two questions. It reacts to small modifications of the questions as well.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">// The example below depicts  two  question-answer pair sr, this time with several examples for the same intent. </t>
-  </si>
-  <si>
     <t>How should I react in case of tantrums</t>
   </si>
   <si>
@@ -349,112 +331,10 @@
     <t>//  Description of the buttons in column C consists of long text, equal sing long text. If more buttons should be displayed, their descriptions are separated by semicolon (;)Popis jednotlivých tlačítek od sebe odděluje středník, každý popis tlačítka začíná krátkým textem, znakem = následovaným dlouhým textem</t>
   </si>
   <si>
-    <t>//Such a description is often unnecessarily complex. If you don't mind that the question "I want to help" chatbot answers anywhere in the dialog, the concept of section and the fourth column are not meant for you.</t>
-  </si>
-  <si>
-    <r>
-      <t>//    By</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Watson Assistant words:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> By specifiing a value in D column we ask to create a GOTO link in a node to the node following the lable.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>//  if the label starts by b_, for example b_agreement, the target node is executed without evaluation of a condition and without waiting for a user input.</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  By Watson Assistant words::</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> b_ means = set the selector of GOTO to body</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">//  if the label starts by c_, for example c_agreement, the condition of the target node is evaluated first. No  user input is collected.  By Watson Assistant words:: c_ means = set the selector of GOTO to condition </t>
   </si>
   <si>
-    <t>// Naming the intents, using the same intent at more Pojmenování intentu a použití stejného intentu na více místech</t>
-  </si>
-  <si>
-    <t>// Example: responding to  "yes" given by user in reply to   "Do you have a headache?"should be different ten "yes" Is reply to  "Do you want an address of the closest hospital?"</t>
-  </si>
-  <si>
     <t xml:space="preserve">//  It is useful to be able to respond to the same sentence differently depending on context. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">// We do not want to restate all the examplesin in two placeces. Instead we name and define the group of input examples once and then use just name at several places. </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">// nemusíte ale popisovat varianty odpovědí vždy znovu, můžete si skupinu vět (tzv intent) označit společným názvem a pak ji používat na více místech. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>By Watson Assistant words</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> this is definition of an  intent.</t>
-    </r>
   </si>
   <si>
     <t>// Intent names start by #. Typically, we use capitals for intent names and replace spaces by underscore.</t>
@@ -863,12 +743,6 @@
     <t xml:space="preserve">// The second column is dedicated to output. It contains a plain text or an optional HTML markup. Default client (clientv2) supports HTML formát. </t>
   </si>
   <si>
-    <t xml:space="preserve"> true and @LIMB:hand</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> true and @LIMB:leg</t>
-  </si>
-  <si>
     <t>#ACHE and @LIMB:hand</t>
   </si>
   <si>
@@ -879,13 +753,193 @@
   </si>
   <si>
     <t>#WHAT_IS and @SUBJECT:XRAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @LIMB:hand</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @LIMB:leg</t>
+  </si>
+  <si>
+    <t>#$ welcome</t>
+  </si>
+  <si>
+    <t>// If one needs to enforce interpretting the text as a condition, prompt the text by a character sequence " #$ " (there is a space after $). This is the way how one can enforce some particular texts e.g "welcome", "true", "false", "anything_else"</t>
+  </si>
+  <si>
+    <t>// to be interpreted the same as understood by Watson Assistant, i.e. to display output as a welcome prompt, always (true), never (false) or if none of the previous conditions was satisfied (anything_else).</t>
+  </si>
+  <si>
+    <t>// Text in the left column must be a condition or a text. One can not combine the two. The condition is just one (while text can have several alternatives).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welcome from this example application </t>
+  </si>
+  <si>
+    <t>// It is not always possible to answer the questions without knowing context. If you want to conduct some steps only if they appear in a particular context, you can describe it in fourth  (D) column by refering to the part, which describes the behivour.</t>
+  </si>
+  <si>
+    <t>//   Section is then introduced by character : followed by the same name</t>
+  </si>
+  <si>
+    <r>
+      <t>//  if the label starts by b_, for example b_agreement, the target node is executed without evaluation of a condition and without waiting for a user input.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  In Watson Assistant words::</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> b_ means = set the selector of GOTO to body</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>// In</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Watson Assistant words</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> this is definition of an  intent.</t>
+    </r>
+  </si>
+  <si>
+    <t>// Naming the intents, using the same intent at more places</t>
+  </si>
+  <si>
+    <t>// Example: responding to  "yes" given by user in reply to   "Do you have a headache?"should be different then if "yes" is a reply to  "Do you want an address of the closest hospital?"</t>
+  </si>
+  <si>
+    <r>
+      <t>//   In</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Watson Assistant words:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> By specifying a value in D column we ask to create a GOTO link in a node to the node following the lable.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>// One should always thing of the T2C sheet as of  a linear sequence of rules (unless expressed otherwise by column D). The rules are checked unless some triggers and next rule is the block below (or the block where we get by specifiing the label in D column).</t>
+  </si>
+  <si>
+    <t>//     One shold make sure that the processing of the rules of the local branch does not spill to next branch .</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">//     Standard way how to ensure it is to conclude each local branch by a rule </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>#$ anything_else</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> which handles the situation when user enters the input which is not handled by any of the rules in the local branch.</t>
+    </r>
+  </si>
+  <si>
+    <t>#$ anything_else</t>
+  </si>
+  <si>
+    <t>Sorry, I do not understand</t>
+  </si>
+  <si>
+    <t>// You write the question to the first column (A) . The required answers is in the second column (B)  . Each pair (question, answer) is separated by empty row</t>
+  </si>
+  <si>
+    <t>// Chat bot described above  is able to answer two questions. It reacts to small modifications of the questions as well.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">// The example below depicts  two  question-answer pairs, this time with several examples for the same intent. </t>
+  </si>
+  <si>
+    <t>// Such a description is often unnecessarily complex. If you don't mind that the question "I want to help" chatbot answers anywhere in the dialog, the concept of section and the fourth column are not meant for you.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">// We do not want to restate all the examples in in two placeces. Instead we name and define the group of input examples once and then use just name at several places. </t>
+  </si>
+  <si>
+    <t>Pardon, nerozumím</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -981,6 +1035,15 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1024,7 +1087,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1046,6 +1109,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1327,10 +1396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D219"/>
+  <dimension ref="A1:D243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="A168" sqref="A168"/>
+    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
+      <selection activeCell="A189" sqref="A189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1338,66 +1407,67 @@
     <col min="1" max="1" width="55.6640625" customWidth="1"/>
     <col min="2" max="2" width="44.44140625" customWidth="1"/>
     <col min="3" max="3" width="92.33203125" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="B3" s="3"/>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>82</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>10</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -1410,47 +1480,47 @@
     </row>
     <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>83</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>84</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -1458,7 +1528,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -1472,17 +1542,17 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -1490,30 +1560,30 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
     </row>
     <row r="33" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
@@ -1523,7 +1593,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1531,38 +1601,38 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D42" s="8"/>
     </row>
@@ -1571,15 +1641,15 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
@@ -1592,46 +1662,46 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" s="9" t="s">
         <v>78</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>79</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>80</v>
+        <v>182</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>81</v>
+        <v>183</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1641,42 +1711,38 @@
       <c r="D56" s="8"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B57" s="8"/>
+      <c r="A57" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>193</v>
+      </c>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>42</v>
-      </c>
+      <c r="A58" s="8"/>
+      <c r="B58" s="8"/>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="8"/>
+      <c r="A59" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
     </row>
-    <row r="60" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="11" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B60" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B60" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>28</v>
-      </c>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="8"/>
@@ -1684,259 +1750,255 @@
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
+    <row r="62" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A62" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>35</v>
-      </c>
+      <c r="A63" s="11"/>
+      <c r="B63" s="9"/>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="8"/>
-      <c r="B64" s="8"/>
+      <c r="A64" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>193</v>
+      </c>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>34</v>
-      </c>
+      <c r="A65" s="8"/>
+      <c r="B65" s="8"/>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
     </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B66" s="8"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+    </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="14" t="s">
-        <v>91</v>
-      </c>
+      <c r="A67" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="8"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="14" t="s">
-        <v>92</v>
-      </c>
+      <c r="A70" s="8"/>
+      <c r="B70" s="8"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="14" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="14"/>
+      <c r="A71" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>100</v>
+      <c r="A73" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="14" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="14"/>
+    </row>
+    <row r="76" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="14" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="14" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="14"/>
+    </row>
+    <row r="79" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="14" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="14"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="14" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B82" s="9"/>
-      <c r="C82" s="9"/>
-      <c r="D82" s="9"/>
+      <c r="A82" s="14" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B83" s="9"/>
-      <c r="C83" s="9"/>
-      <c r="D83" s="9"/>
+      <c r="A83" s="14"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B84" s="9"/>
-      <c r="C84" s="9"/>
-      <c r="D84" s="9"/>
+      <c r="A84" s="12" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="9"/>
-      <c r="B85" s="9"/>
-      <c r="C85" s="9"/>
-      <c r="D85" s="9"/>
+      <c r="A85" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B86" s="8"/>
-      <c r="C86" s="8"/>
-      <c r="D86" s="8"/>
+      <c r="A86" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B87" s="8"/>
-      <c r="C87" s="8"/>
-      <c r="D87" s="8"/>
+      <c r="A87" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B88" s="8"/>
-      <c r="C88" s="8"/>
-      <c r="D88" s="8"/>
+      <c r="A88" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B89" s="8"/>
-      <c r="C89" s="8"/>
-      <c r="D89" s="8"/>
+      <c r="A89" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" s="8" t="s">
+      <c r="A93" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B93" s="9"/>
+      <c r="C93" s="9"/>
+      <c r="D93" s="9"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B94" s="9"/>
+      <c r="C94" s="9"/>
+      <c r="D94" s="9"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B95" s="9"/>
+      <c r="C95" s="9"/>
+      <c r="D95" s="9"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="9"/>
+      <c r="B96" s="9"/>
+      <c r="C96" s="9"/>
+      <c r="D96" s="9"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B93" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C93" s="8"/>
-      <c r="D93" s="8"/>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" s="8"/>
-      <c r="B94" s="8"/>
-      <c r="C94" s="8"/>
-      <c r="D94" s="8"/>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B95" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C95" s="8"/>
-      <c r="D95" s="8"/>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>103</v>
-      </c>
+      <c r="B97" s="8"/>
+      <c r="C97" s="8"/>
+      <c r="D97" s="8"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B98" s="8"/>
+      <c r="C98" s="8"/>
+      <c r="D98" s="8"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="B99" s="8" t="s">
-        <v>52</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="B99" s="8"/>
       <c r="C99" s="8"/>
-      <c r="D99" s="8" t="s">
-        <v>111</v>
-      </c>
+      <c r="D99" s="8"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="8" t="s">
-        <v>105</v>
+        <v>49</v>
       </c>
       <c r="B100" s="8"/>
       <c r="C100" s="8"/>
       <c r="D100" s="8"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A101" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="B101" s="8"/>
-      <c r="C101" s="8"/>
-      <c r="D101" s="8"/>
-    </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A102" s="8"/>
-      <c r="B102" s="8"/>
-      <c r="C102" s="8"/>
-      <c r="D102" s="8"/>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A103" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="B103" s="8"/>
-      <c r="C103" s="8"/>
-      <c r="D103" s="8"/>
+      <c r="A102" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>109</v>
+        <v>50</v>
       </c>
       <c r="C104" s="8"/>
-      <c r="D104" s="8" t="s">
-        <v>110</v>
-      </c>
+      <c r="D104" s="8"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="8"/>
@@ -1946,10 +2008,10 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="C106" s="8"/>
       <c r="D106" s="8"/>
@@ -1960,96 +2022,132 @@
       <c r="C107" s="8"/>
       <c r="D107" s="8"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A108" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="B108" s="8"/>
+    <row r="108" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="B108" s="9" t="s">
+        <v>193</v>
+      </c>
       <c r="C108" s="8"/>
       <c r="D108" s="8"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A109" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B109" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="C109" s="8"/>
-      <c r="D109" s="8"/>
-    </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A110" s="8"/>
-      <c r="B110" s="8"/>
-      <c r="C110" s="8"/>
-      <c r="D110" s="8"/>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A111" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B111" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C111" s="8"/>
-      <c r="D111" s="8"/>
+      <c r="A110" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B112" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C112" s="8"/>
+      <c r="D112" s="8" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
-        <v>117</v>
-      </c>
+      <c r="A113" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B113" s="8"/>
+      <c r="C113" s="8"/>
+      <c r="D113" s="8"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
-        <v>118</v>
-      </c>
+      <c r="A114" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B114" s="8"/>
+      <c r="C114" s="8"/>
+      <c r="D114" s="8"/>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" s="8"/>
+      <c r="B115" s="8"/>
+      <c r="C115" s="8"/>
+      <c r="D115" s="8"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
-        <v>116</v>
-      </c>
+      <c r="A116" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="B116" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C116" s="8"/>
+      <c r="D116" s="8"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A117" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B117" s="8" t="s">
-        <v>115</v>
-      </c>
+      <c r="A117" s="8"/>
+      <c r="B117" s="8"/>
       <c r="C117" s="8"/>
       <c r="D117" s="8"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="8" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="B118" s="8"/>
       <c r="C118" s="8"/>
       <c r="D118" s="8"/>
     </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B119" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C119" s="8"/>
+      <c r="D119" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A120" s="12" t="s">
-        <v>1</v>
-      </c>
+      <c r="A120" s="8"/>
+      <c r="B120" s="8"/>
+      <c r="C120" s="8"/>
+      <c r="D120" s="8"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A121" s="16" t="s">
-        <v>156</v>
-      </c>
+      <c r="A121" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C121" s="8"/>
+      <c r="D121" s="8"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
-        <v>154</v>
-      </c>
+      <c r="A122" s="8"/>
+      <c r="B122" s="8"/>
+      <c r="C122" s="8"/>
+      <c r="D122" s="8"/>
+    </row>
+    <row r="123" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="B123" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C123" s="8"/>
+      <c r="D123" s="8"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124" s="8"/>
+      <c r="B124" s="8"/>
+      <c r="C124" s="8"/>
+      <c r="D124" s="8"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="8" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
       <c r="B125" s="8"/>
       <c r="C125" s="8"/>
@@ -2057,114 +2155,137 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="B126" s="8"/>
+        <v>43</v>
+      </c>
+      <c r="B126" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="C126" s="8"/>
       <c r="D126" s="8"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A127" s="8" t="s">
-        <v>157</v>
-      </c>
+      <c r="A127" s="8"/>
       <c r="B127" s="8"/>
       <c r="C127" s="8"/>
       <c r="D127" s="8"/>
     </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B128" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C128" s="8"/>
+      <c r="D128" s="8"/>
+    </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
-        <v>158</v>
-      </c>
+      <c r="A129" s="8"/>
+      <c r="B129" s="8"/>
+      <c r="C129" s="8"/>
+      <c r="D129" s="8"/>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A130" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="B130" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C130" s="8"/>
+      <c r="D130" s="8"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A131" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B131" s="8"/>
-      <c r="C131" s="8"/>
-      <c r="D131" s="8"/>
+      <c r="A131" s="17"/>
+      <c r="B131" s="18"/>
+      <c r="C131" s="13"/>
+      <c r="D131" s="13"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A132" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B132" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="C132" s="8"/>
-      <c r="D132" s="8"/>
+      <c r="A132" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A133" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="B133" s="8"/>
-      <c r="C133" s="8"/>
-      <c r="D133" s="8"/>
+      <c r="A133" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>159</v>
-      </c>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A136" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B136" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C136" s="8"/>
+      <c r="D136" s="8"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="B137" s="8" t="s">
-        <v>57</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="B137" s="8"/>
       <c r="C137" s="8"/>
       <c r="D137" s="8"/>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A139" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="B139" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C139" s="8"/>
-      <c r="D139" s="8"/>
+      <c r="A139" s="12" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A140" t="s">
-        <v>166</v>
+      <c r="A140" s="16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A143" t="s">
-        <v>161</v>
-      </c>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A144" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B144" s="8"/>
+      <c r="C144" s="8"/>
+      <c r="D144" s="8"/>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="B145" s="8" t="s">
-        <v>57</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="B145" s="8"/>
       <c r="C145" s="8"/>
       <c r="D145" s="8"/>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A147" t="s">
-        <v>162</v>
-      </c>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A146" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B146" s="8"/>
+      <c r="C146" s="8"/>
+      <c r="D146" s="8"/>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B150" s="8"/>
       <c r="C150" s="8"/>
@@ -2172,400 +2293,504 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B151" s="8"/>
+        <v>107</v>
+      </c>
+      <c r="B151" s="8" t="s">
+        <v>109</v>
+      </c>
       <c r="C151" s="8"/>
       <c r="D151" s="8"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="8" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
       <c r="B152" s="8"/>
       <c r="C152" s="8"/>
       <c r="D152" s="8"/>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A153" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B153" s="8"/>
-      <c r="C153" s="8"/>
-      <c r="D153" s="8"/>
-    </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A154" s="8"/>
-      <c r="B154" s="8"/>
-      <c r="C154" s="8"/>
-      <c r="D154" s="8"/>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A155" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B155" s="8"/>
-      <c r="C155" s="8"/>
-      <c r="D155" s="8"/>
+      <c r="A154" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B156" s="8"/>
+        <v>175</v>
+      </c>
+      <c r="B156" s="8" t="s">
+        <v>56</v>
+      </c>
       <c r="C156" s="8"/>
       <c r="D156" s="8"/>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A157" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="B157" s="8"/>
-      <c r="C157" s="8"/>
-      <c r="D157" s="8"/>
-    </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A158" s="8"/>
-      <c r="B158" s="8"/>
+      <c r="A158" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B158" s="8" t="s">
+        <v>57</v>
+      </c>
       <c r="C158" s="8"/>
       <c r="D158" s="8"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A159" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="B159" s="8" t="s">
+      <c r="A159" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A164" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B164" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C164" s="8"/>
+      <c r="D164" s="8"/>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
         <v>150</v>
       </c>
-      <c r="C159" s="8"/>
-      <c r="D159" s="8"/>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A160" s="8"/>
-      <c r="B160" s="8"/>
-      <c r="C160" s="8"/>
-      <c r="D160" s="8"/>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A161" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="B161" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="C161" s="8"/>
-      <c r="D161" s="8"/>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A163" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A165" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="B165" s="8"/>
-      <c r="C165" s="8"/>
-      <c r="D165" s="8"/>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A166" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B166" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="C166" s="8"/>
-      <c r="D166" s="8"/>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A167" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="B167" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="C167" s="8"/>
-      <c r="D167" s="8"/>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A169" s="14" t="s">
-        <v>126</v>
-      </c>
+      <c r="A169" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B169" s="8"/>
+      <c r="C169" s="8"/>
+      <c r="D169" s="8"/>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A170" s="14" t="s">
-        <v>183</v>
-      </c>
+      <c r="A170" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B170" s="8"/>
+      <c r="C170" s="8"/>
+      <c r="D170" s="8"/>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A171" s="14" t="s">
-        <v>179</v>
-      </c>
+      <c r="A171" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B171" s="8"/>
+      <c r="C171" s="8"/>
+      <c r="D171" s="8"/>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="B172" s="8" t="s">
-        <v>176</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="B172" s="8"/>
       <c r="C172" s="8"/>
       <c r="D172" s="8"/>
     </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A173" s="8"/>
+      <c r="B173" s="8"/>
+      <c r="C173" s="8"/>
+      <c r="D173" s="8"/>
+    </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A174" s="14" t="s">
-        <v>182</v>
-      </c>
+      <c r="A174" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B174" s="8"/>
+      <c r="C174" s="8"/>
+      <c r="D174" s="8"/>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A175" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B175" s="8"/>
+      <c r="C175" s="8"/>
+      <c r="D175" s="8"/>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="B176" s="8" t="s">
-        <v>181</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="B176" s="8"/>
       <c r="C176" s="8"/>
       <c r="D176" s="8"/>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A177" s="14" t="s">
+      <c r="A177" s="8"/>
+      <c r="B177" s="8"/>
+      <c r="C177" s="8"/>
+      <c r="D177" s="8"/>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A178" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B178" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C178" s="8"/>
+      <c r="D178" s="8"/>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A179" s="8"/>
+      <c r="B179" s="8"/>
+      <c r="C179" s="8"/>
+      <c r="D179" s="8"/>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A180" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B180" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C180" s="8"/>
+      <c r="D180" s="8"/>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A184" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B184" s="8"/>
+      <c r="C184" s="8"/>
+      <c r="D184" s="8"/>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A185" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B185" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C185" s="8"/>
+      <c r="D185" s="8"/>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A186" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B186" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C186" s="8"/>
+      <c r="D186" s="8"/>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
         <v>180</v>
       </c>
-      <c r="B177" s="14"/>
-    </row>
-    <row r="178" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A179" s="14" t="s">
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A180" s="14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A181" s="14" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A182" s="14" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A183" s="14" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A184" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A185" s="14" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A186" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A187" s="14" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A188" s="14" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A189" s="14" t="s">
-        <v>149</v>
-      </c>
-    </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A190" s="14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A191" s="8" t="s">
-        <v>123</v>
+        <v>177</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="C191" s="8"/>
-      <c r="D191" s="8"/>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A192" s="14" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A193" s="14"/>
+      <c r="A193" s="14" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" s="14" t="s">
-        <v>127</v>
+        <v>170</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" s="14" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" s="8" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="B196" s="8" t="s">
-        <v>133</v>
+        <v>163</v>
       </c>
       <c r="C196" s="8"/>
       <c r="D196" s="8"/>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A197" s="13"/>
-      <c r="B197" s="13"/>
-      <c r="C197" s="13"/>
-      <c r="D197" s="13"/>
-    </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A198" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="B198" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="C198" s="13"/>
-      <c r="D198" s="13"/>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A199" s="13"/>
-      <c r="B199" s="13"/>
-      <c r="C199" s="13"/>
-      <c r="D199" s="13"/>
+      <c r="A198" s="14" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A200" s="14" t="s">
-        <v>137</v>
-      </c>
+      <c r="A200" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B200" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C200" s="8"/>
+      <c r="D200" s="8"/>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A201" s="14"/>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A202" s="14" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="203" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A201" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="B201" s="14"/>
+    </row>
+    <row r="202" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" s="14" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" s="14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="205" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A205" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="B205" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="C205" s="13"/>
-      <c r="D205" s="13"/>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A205" s="14" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A206" s="14"/>
+      <c r="A206" s="14" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" s="14" t="s">
-        <v>168</v>
+        <v>130</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" s="14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="209" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A209" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="B209" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="C209" s="13"/>
-      <c r="D209" s="13"/>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A209" s="14" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A210" s="14"/>
+      <c r="A210" s="14" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" s="14" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" s="14" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" s="14" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" s="14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="215" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A215" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="B215" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A215" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B215" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C215" s="8"/>
+      <c r="D215" s="8"/>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A216" s="14" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A217" s="14"/>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A218" s="14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A219" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A220" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B220" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C220" s="8"/>
+      <c r="D220" s="8"/>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A221" s="13"/>
+      <c r="B221" s="13"/>
+      <c r="C221" s="13"/>
+      <c r="D221" s="13"/>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A222" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B222" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C222" s="13"/>
+      <c r="D222" s="13"/>
+    </row>
+    <row r="223" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A224" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A225" s="14"/>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A226" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A227" s="14" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A228" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A229" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B229" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C229" s="13"/>
+      <c r="D229" s="13"/>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A230" s="14"/>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A231" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A232" s="14" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A233" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="B233" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="C233" s="13"/>
+      <c r="D233" s="13"/>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A234" s="14"/>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A235" s="14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A236" s="14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A237" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A238" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A239" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B239" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C239" s="13"/>
+      <c r="D239" s="13"/>
+    </row>
+    <row r="240" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="241" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A241" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C215" s="13"/>
-      <c r="D215" s="13"/>
-    </row>
-    <row r="216" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="217" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A217" s="13" t="s">
+      <c r="B241" s="13"/>
+      <c r="C241" s="13"/>
+      <c r="D241" s="13"/>
+    </row>
+    <row r="242" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A242" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="B217" s="13"/>
-      <c r="C217" s="13"/>
-      <c r="D217" s="13"/>
-    </row>
-    <row r="218" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A218" s="13" t="s">
+      <c r="B242" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B218" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C218" s="13"/>
-      <c r="D218" s="13"/>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A219" s="14"/>
+      <c r="C242" s="13"/>
+      <c r="D242" s="13"/>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A243" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>